<commit_message>
update the course website with some more steps
</commit_message>
<xml_diff>
--- a/binary files/Data 301 Course map.xlsx
+++ b/binary files/Data 301 Course map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/firasm/Sync/Teaching/ubco/data301_course/binary files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365FABC3-567F-1548-8D86-64A0C0353034}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4015A1D6-D06B-AD4C-9F12-B78BC02DD106}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" activeTab="2" xr2:uid="{DB8961C7-4B63-584D-B429-6BEA620936BA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="91">
   <si>
     <t>Week</t>
   </si>
@@ -1541,7 +1541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69171063-8EC6-8842-B21B-7D5A50E96CE9}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="157" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="157" workbookViewId="0">
       <selection activeCell="G14" sqref="A1:G14"/>
     </sheetView>
   </sheetViews>
@@ -1587,6 +1587,9 @@
       <c r="C2" t="s">
         <v>68</v>
       </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
       <c r="E2" t="s">
         <v>69</v>
       </c>

</xml_diff>